<commit_message>
working model, correctly calculates difference in percentages
</commit_message>
<xml_diff>
--- a/input/Rate Table per ton.xlsx
+++ b/input/Rate Table per ton.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fusio\Desktop\shoutlines_project\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pankaj\Desktop\shortlines_project\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE545684-EA9E-4073-9FBB-2C14FF23105B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,8 +52,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -115,10 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -399,23 +399,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,117 +435,132 @@
         <v>400</v>
       </c>
       <c r="F1" s="2">
+        <v>600</v>
+      </c>
+      <c r="G1" s="2">
         <v>800</v>
       </c>
-      <c r="G1" s="2">
+      <c r="H1" s="2">
         <v>1000</v>
       </c>
-      <c r="H1" s="2">
+      <c r="I1" s="2">
         <v>1200</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>9.1690000000000005</v>
+        <v>9.17</v>
       </c>
       <c r="C2" s="4">
-        <v>16.465199999999999</v>
+        <v>16.22</v>
       </c>
       <c r="D2" s="4">
-        <v>31.048300000000001</v>
+        <v>30.56</v>
       </c>
       <c r="E2" s="4">
-        <v>68.331599999999995</v>
+        <v>67.28</v>
       </c>
       <c r="F2" s="4">
-        <v>134.3587</v>
+        <v>99.63</v>
       </c>
       <c r="G2" s="4">
-        <v>167.82230000000001</v>
+        <v>132.56</v>
       </c>
       <c r="H2" s="4">
-        <v>200.98589999999999</v>
+        <v>165.2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>197.84</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>7.1285999999999996</v>
+        <v>7.83</v>
       </c>
       <c r="C3" s="4">
-        <v>12.813599999999999</v>
+        <v>12.81</v>
       </c>
       <c r="D3" s="4">
-        <v>24.183599999999998</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4">
-        <v>52.412100000000002</v>
+        <v>52.41</v>
       </c>
       <c r="F3" s="4">
-        <v>103.3098</v>
+        <v>77.86</v>
       </c>
       <c r="G3" s="4">
-        <v>128.7586</v>
+        <v>103.31</v>
       </c>
       <c r="H3" s="4">
-        <v>154.20740000000001</v>
+        <v>128.76</v>
+      </c>
+      <c r="I3" s="4">
+        <v>154.21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>7.8265000000000002</v>
+        <v>7.83</v>
       </c>
       <c r="C4" s="4">
-        <v>14.060499999999999</v>
+        <v>14.06</v>
       </c>
       <c r="D4" s="4">
-        <v>26.528400000000001</v>
+        <v>26.53</v>
       </c>
       <c r="E4" s="4">
-        <v>57.793399999999998</v>
+        <v>57.79</v>
       </c>
       <c r="F4" s="4">
-        <v>113.90770000000001</v>
+        <v>85.85</v>
       </c>
       <c r="G4" s="4">
-        <v>141.9648</v>
+        <v>113.91</v>
       </c>
       <c r="H4" s="4">
-        <v>170.02189999999999</v>
+        <v>141.96</v>
+      </c>
+      <c r="I4" s="4">
+        <v>170.02</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>8.0260999999999996</v>
+        <v>8.01</v>
       </c>
       <c r="C5" s="4">
-        <v>14.4747</v>
+        <v>14.44</v>
       </c>
       <c r="D5" s="4">
-        <v>27.3719</v>
+        <v>27.3</v>
       </c>
       <c r="E5" s="4">
-        <v>59.5246</v>
+        <v>59.37</v>
       </c>
       <c r="F5" s="4">
-        <v>117.3867</v>
+        <v>88.23</v>
       </c>
       <c r="G5" s="4">
-        <v>146.31780000000001</v>
+        <v>117.09</v>
       </c>
       <c r="H5" s="4">
-        <v>175.24879999999999</v>
+        <v>145.94</v>
+      </c>
+      <c r="I5" s="4">
+        <v>174.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>